<commit_message>
Nov 03, 2022 08:29PM
</commit_message>
<xml_diff>
--- a/_CaltexGoPH/src/test/resources/Local Datasheets/OnBoarding_LandingPage.xlsx
+++ b/_CaltexGoPH/src/test/resources/Local Datasheets/OnBoarding_LandingPage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mobile Automation\Git Repository\CaltexGoPH\_CaltexGoPH\src\test\resources\Local Datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{753F20C5-FE22-47C5-9AB8-E594D37D06E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472684BC-E5C9-41FF-9582-F3A665FA4F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Country Options</t>
   </si>
@@ -33,10 +33,25 @@
     <t>Australia;Malaysia;Philippines;Thailand</t>
   </si>
   <si>
-    <t>Language Options</t>
-  </si>
-  <si>
     <t>English</t>
+  </si>
+  <si>
+    <t>Language Options_Australia</t>
+  </si>
+  <si>
+    <t>Language Options_Malaysia</t>
+  </si>
+  <si>
+    <t>English;Bahasa Melayu</t>
+  </si>
+  <si>
+    <t>Language Options_Philippines</t>
+  </si>
+  <si>
+    <t>Language Options_Thailand</t>
+  </si>
+  <si>
+    <t>อังกฤษ;ไทย</t>
   </si>
 </sst>
 </file>
@@ -357,33 +372,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="1" width="33.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="24.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>